<commit_message>
GPA, MajorGPA, TotalCredits and Speculated GPA added
</commit_message>
<xml_diff>
--- a/Academic_Transcript/Grades-15BCE1339.xlsx
+++ b/Academic_Transcript/Grades-15BCE1339.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="116">
   <si>
     <t>S.No.</t>
   </si>
@@ -61,21 +61,42 @@
     <t>23-Dec-2015</t>
   </si>
   <si>
+    <t>CHY1002</t>
+  </si>
+  <si>
+    <t>Environmental Sciences</t>
+  </si>
+  <si>
+    <t>Embedded - Theory &amp; Project</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>May-2016</t>
+  </si>
+  <si>
+    <t>10-Jun-2016</t>
+  </si>
+  <si>
+    <t>CSE1001</t>
+  </si>
+  <si>
+    <t>Problem Solving and Programming</t>
+  </si>
+  <si>
+    <t>Lab Only</t>
+  </si>
+  <si>
     <t>CSE1002</t>
   </si>
   <si>
     <t>Problem Solving with Object Oriented Programming</t>
   </si>
   <si>
-    <t>Lab Only</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>May-2016</t>
-  </si>
-  <si>
     <t>14-Jun-2016</t>
   </si>
   <si>
@@ -88,9 +109,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>10-Jun-2016</t>
-  </si>
-  <si>
     <t>CSE1004</t>
   </si>
   <si>
@@ -124,9 +142,6 @@
     <t>Theory of Computation and Compiler Design</t>
   </si>
   <si>
-    <t>Embedded - Theory &amp; Project</t>
-  </si>
-  <si>
     <t>CSE2003</t>
   </si>
   <si>
@@ -136,6 +151,18 @@
     <t>13-Jun-2016</t>
   </si>
   <si>
+    <t>CSE2004</t>
+  </si>
+  <si>
+    <t>Database Management Systems</t>
+  </si>
+  <si>
+    <t>CSE2005</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
     <t>CSE2006</t>
   </si>
   <si>
@@ -181,6 +208,21 @@
     <t>Web Mining</t>
   </si>
   <si>
+    <t>CSE3099</t>
+  </si>
+  <si>
+    <t>Industrial Internship</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10-Jan-2018</t>
+  </si>
+  <si>
     <t>CSE4001</t>
   </si>
   <si>
@@ -214,15 +256,18 @@
     <t>English for Engineers</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>GER1001</t>
   </si>
   <si>
     <t>Basic German</t>
   </si>
   <si>
+    <t>HUM1021</t>
+  </si>
+  <si>
+    <t>Ethics and Values</t>
+  </si>
+  <si>
     <t>HUM1022</t>
   </si>
   <si>
@@ -257,6 +302,12 @@
   </si>
   <si>
     <t>Applied Linear Algebra</t>
+  </si>
+  <si>
+    <t>MGT1022</t>
+  </si>
+  <si>
+    <t>Lean Start-up Management</t>
   </si>
   <si>
     <t>MGT1027</t>
@@ -688,25 +739,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>